<commit_message>
Added logic to replace all 0's with 1's during data collection
</commit_message>
<xml_diff>
--- a/output/report.xlsx
+++ b/output/report.xlsx
@@ -7,13 +7,15 @@
   </bookViews>
   <sheets>
     <sheet name="Stocks Found" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="ANFIF" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="NOBDF" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="URPTF" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="CCM" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="TNP" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="KFY" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="PLUG" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="WTER" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="AUSAF" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="ANFIF" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="NOBDF" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="CCM" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="SARSF" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="VIZSF" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="KEGX" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="HSCHF" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -457,7 +459,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,17 +525,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ANFIF</t>
+          <t>WTER</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Amira Nature Foods Ltd</t>
+          <t>Alkaline Water Company Inc</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2021-06-22T12:30:00.000Z</t>
+          <t>2021-07-02T12:30:00.000Z</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -561,22 +563,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NOBDF</t>
+          <t>AUSAF</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>North Bud Farms Inc</t>
+          <t>Australis Capital Inc</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2021-06-22T19:30:00.000Z</t>
+          <t>2021-07-03T03:00:00.000Z</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>BMO</t>
+          <t>AMC</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -599,22 +601,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>URPTF</t>
+          <t>ANFIF</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Uranium Participation Corp</t>
+          <t>Amira Nature Foods Ltd</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2021-06-22T20:00:00.000Z</t>
+          <t>2021-07-02T12:30:00.000Z</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>AMC</t>
+          <t>BMO</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -637,22 +639,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CCM</t>
+          <t>NOBDF</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Concord Medical Services Holdings Ltd</t>
+          <t>North Bud Farms Inc</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2021-06-22T20:00:00.000Z</t>
+          <t>2021-07-02T19:30:00.000Z</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>AMC</t>
+          <t>BMO</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -675,22 +677,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TNP</t>
+          <t>CCM</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Tsakos Energy Navigation Ltd</t>
+          <t>Concord Medical Services Holdings Ltd</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2021-06-22T12:30:00.000Z</t>
+          <t>2021-07-02T20:00:00.000Z</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>BMO</t>
+          <t>AMC</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -713,26 +715,23 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>KFY</t>
+          <t>SARSF</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Korn Ferry</t>
+          <t>Canada House Cannabis Group Inc</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2021-06-22T12:30:00.000Z</t>
+          <t>2021-07-02T12:30:00.000Z</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>BMO</t>
         </is>
-      </c>
-      <c r="F7" t="n">
-        <v>0.98</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -754,26 +753,23 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>PLUG</t>
+          <t>VIZSF</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Plug Power Inc</t>
+          <t>Vizsla Silver Corp</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2021-06-22T12:30:00.000Z</t>
+          <t>2021-07-02T20:00:00.000Z</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>BMO</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>-0.08</v>
+          <t>AMC</t>
+        </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -789,8 +785,488 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>KEGX</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Key Energy Services Inc</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2021-07-02T10:59:00.000Z</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>TNS</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>EDT</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>-14400000</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>EQUITY</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>HSCHF</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>H-Source Holdings Ltd</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2021-07-02T20:00:00.000Z</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>AMC</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>EDT</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>-14400000</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>EQUITY</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Current</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>1YA</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>2YA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>sharePrice</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0.09039999999999999</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.09039999999999999</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.09039999999999999</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>marketCap</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>10634656</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10634656</v>
+      </c>
+      <c r="D3" t="n">
+        <v>10634656</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>totalRevenue</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>619808</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1291058</v>
+      </c>
+      <c r="D4" t="n">
+        <v>309244</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>grossProfit</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-984081</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-1096562</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-1184732</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>operatingIncome</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-2459404</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-2984350</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-2677024</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>netIncome</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-2934024</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-3054090</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-2667674</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>ebit</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-2459404</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-2984350</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-2677024</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>netReceivables</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>75631</v>
+      </c>
+      <c r="C9" t="n">
+        <v>207676</v>
+      </c>
+      <c r="D9" t="n">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>inventory</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2674</v>
+      </c>
+      <c r="C10" t="n">
+        <v>111460</v>
+      </c>
+      <c r="D10" t="n">
+        <v>12592</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>currentAssets</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>206981</v>
+      </c>
+      <c r="C11" t="n">
+        <v>632098</v>
+      </c>
+      <c r="D11" t="n">
+        <v>371983</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>totalAssets</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>947535</v>
+      </c>
+      <c r="C12" t="n">
+        <v>924129</v>
+      </c>
+      <c r="D12" t="n">
+        <v>847990</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>currentLiabilities</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>3876091</v>
+      </c>
+      <c r="C13" t="n">
+        <v>959711</v>
+      </c>
+      <c r="D13" t="n">
+        <v>242475</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>longTermDebt</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>totalLiabilities</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>3876091</v>
+      </c>
+      <c r="C15" t="n">
+        <v>959711</v>
+      </c>
+      <c r="D15" t="n">
+        <v>242475</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>retainedEarnings</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-13854098</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-10920074</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-7865984</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>liabilitiesAndEquity</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>947535</v>
+      </c>
+      <c r="C17" t="n">
+        <v>924129</v>
+      </c>
+      <c r="D17" t="n">
+        <v>847990</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>dividends</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>shareIssuance</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2093634</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2094901</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>shareBuyback</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>1</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>operatingCashFlow</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-1437851</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-2472075</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-2578115</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>capitalExpenditure</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>depreciation</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>13004</v>
+      </c>
+      <c r="C23" t="n">
+        <v>11878</v>
+      </c>
+      <c r="D23" t="n">
+        <v>10663</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>eps</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-0.02</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -832,13 +1308,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>1.46</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>1.46</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="3">
@@ -848,13 +1324,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>130976600</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>130976600</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>130976600</v>
       </c>
     </row>
     <row r="4">
@@ -864,13 +1340,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>41142443</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>32199528</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>19812199</v>
       </c>
     </row>
     <row r="5">
@@ -880,13 +1356,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>16839569</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>12946760</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>8125182</v>
       </c>
     </row>
     <row r="6">
@@ -896,13 +1372,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>-14378063</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>-8063371</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>-5930063</v>
       </c>
     </row>
     <row r="7">
@@ -912,13 +1388,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>-14826821</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>-8617565</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>-6687280</v>
       </c>
     </row>
     <row r="8">
@@ -928,13 +1404,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>-14378063</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>-8063371</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>-5930063</v>
       </c>
     </row>
     <row r="9">
@@ -944,13 +1420,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>4917081</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>3068181</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>2599095</v>
       </c>
     </row>
     <row r="10">
@@ -960,13 +1436,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>2919860</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>2058012</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>1002020</v>
       </c>
     </row>
     <row r="11">
@@ -976,13 +1452,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>14183215</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>16537343</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>4886491</v>
       </c>
     </row>
     <row r="12">
@@ -992,13 +1468,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>15605796</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>18482608</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>6056126</v>
       </c>
     </row>
     <row r="13">
@@ -1008,13 +1484,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>13983663</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>7125695</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>5595885</v>
       </c>
     </row>
     <row r="14">
@@ -1040,13 +1516,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>13983663</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>7125695</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>5595885</v>
       </c>
     </row>
     <row r="16">
@@ -1056,13 +1532,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>-53521700</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>-38694879</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>-30077314</v>
       </c>
     </row>
     <row r="17">
@@ -1072,13 +1548,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>15605796</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>18482608</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>6056126</v>
       </c>
     </row>
     <row r="18">
@@ -1104,13 +1580,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>3500486</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>19120777</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>2450000</v>
       </c>
     </row>
     <row r="20">
@@ -1136,13 +1612,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>-13642636</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>-8128613</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>-2625849</v>
       </c>
     </row>
     <row r="22">
@@ -1152,13 +1628,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>-488557</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>-1356299</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>-317855</v>
       </c>
     </row>
     <row r="23">
@@ -1168,13 +1644,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>1023237</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>580669</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>418777</v>
       </c>
     </row>
     <row r="24">
@@ -1184,13 +1660,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>-0.257</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>-0.257</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>-0.257</v>
       </c>
     </row>
   </sheetData>
@@ -1236,13 +1712,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.2767</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0.2767</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.2767</v>
       </c>
     </row>
     <row r="3">
@@ -1252,13 +1728,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>48908936</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>48908936</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>48908936</v>
       </c>
     </row>
     <row r="4">
@@ -1268,10 +1744,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>221482</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>129759</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
@@ -1284,10 +1760,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>221482</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>129759</v>
       </c>
       <c r="D5" t="n">
         <v>1</v>
@@ -1300,13 +1776,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>-14176051</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>-3758654</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>-1040</v>
       </c>
     </row>
     <row r="7">
@@ -1316,13 +1792,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>-23342148</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>-4171210</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>-42697</v>
       </c>
     </row>
     <row r="8">
@@ -1332,13 +1808,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>-14176051</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>-3758654</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>-1040</v>
       </c>
     </row>
     <row r="9">
@@ -1348,13 +1824,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>433736</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>398183</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>3008556</v>
       </c>
     </row>
     <row r="10">
@@ -1380,13 +1856,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>23715598</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>30885144</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>3010401</v>
       </c>
     </row>
     <row r="12">
@@ -1396,13 +1872,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>63700339</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>65051386</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>3010501</v>
       </c>
     </row>
     <row r="13">
@@ -1412,13 +1888,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>3875472</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>1633184</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>3173423</v>
       </c>
     </row>
     <row r="14">
@@ -1444,13 +1920,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>5934315</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>4377063</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>3173423</v>
       </c>
     </row>
     <row r="16">
@@ -1460,13 +1936,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>-27676380</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>-4334232</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>-163022</v>
       </c>
     </row>
     <row r="17">
@@ -1476,13 +1952,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>63700339</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>65051386</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>3010501</v>
       </c>
     </row>
     <row r="18">
@@ -1508,13 +1984,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>2688756</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>51886684</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>51886684</v>
       </c>
     </row>
     <row r="20">
@@ -1524,13 +2000,13 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>-287280</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>-287280</v>
       </c>
       <c r="D20" t="n">
-        <v>1</v>
+        <v>-287280</v>
       </c>
     </row>
     <row r="21">
@@ -1540,13 +2016,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>-8323275</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>-2805979</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>-619</v>
       </c>
     </row>
     <row r="22">
@@ -1556,13 +2032,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>-704576</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>-130641</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>-130641</v>
       </c>
     </row>
     <row r="23">
@@ -1572,13 +2048,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>601245</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>10025</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>10025</v>
       </c>
     </row>
     <row r="24">
@@ -1588,13 +2064,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>-0.183</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>-0.183</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>-0.183</v>
       </c>
     </row>
   </sheetData>
@@ -1640,13 +2116,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>1.81</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>1.81</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="3">
@@ -1656,13 +2132,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>4020172</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>4020172</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>4020172</v>
       </c>
     </row>
     <row r="4">
@@ -1672,13 +2148,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>64597621</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>418933307</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>551879799</v>
       </c>
     </row>
     <row r="5">
@@ -1688,13 +2164,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>-135219140</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>73273021</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>94862433</v>
       </c>
     </row>
     <row r="6">
@@ -1704,13 +2180,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>-325418902</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>51313075</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>68926889</v>
       </c>
     </row>
     <row r="7">
@@ -1720,13 +2196,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>-304911721</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>-78222174</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>25087388</v>
       </c>
     </row>
     <row r="8">
@@ -1736,13 +2212,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>-325418902</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>51313075</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>68926889</v>
       </c>
     </row>
     <row r="9">
@@ -1752,13 +2228,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>828776</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>259959073</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>210557628</v>
       </c>
     </row>
     <row r="10">
@@ -1768,13 +2244,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>1172369</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>161278863</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>273063839</v>
       </c>
     </row>
     <row r="11">
@@ -1784,13 +2260,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>23478028</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>492312312</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>552972603</v>
       </c>
     </row>
     <row r="12">
@@ -1800,13 +2276,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>26156565</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>512826507</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>574605215</v>
       </c>
     </row>
     <row r="13">
@@ -1816,13 +2292,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>13356166</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>270101820</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>266556835</v>
       </c>
     </row>
     <row r="14">
@@ -1832,13 +2308,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>27580975</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>27430</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>48743</v>
       </c>
     </row>
     <row r="15">
@@ -1848,13 +2324,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>41228571</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>271217631</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>271380794</v>
       </c>
     </row>
     <row r="16">
@@ -1864,13 +2340,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>-58911829</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>91815016</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>167424244</v>
       </c>
     </row>
     <row r="17">
@@ -1880,13 +2356,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>26156565</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>512826507</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>574605215</v>
       </c>
     </row>
     <row r="18">
@@ -1944,13 +2420,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>-169425631</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>-28379041</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>5787060</v>
       </c>
     </row>
     <row r="22">
@@ -1963,10 +2439,10 @@
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>-442568</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>-71885</v>
       </c>
     </row>
     <row r="23">
@@ -1976,13 +2452,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>764640</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>1617118</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>1778968</v>
       </c>
     </row>
     <row r="24">
@@ -2044,13 +2520,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="3">
@@ -2060,13 +2536,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>6344190</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>6344190</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>6344190</v>
       </c>
     </row>
     <row r="4">
@@ -2108,7 +2584,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>-1815482</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -2124,7 +2600,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>-1804540</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -2140,7 +2616,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>-1815482</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
@@ -2156,7 +2632,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>302553</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
@@ -2188,7 +2664,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>4515146</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
@@ -2204,7 +2680,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>7691156</v>
       </c>
       <c r="C12" t="n">
         <v>1</v>
@@ -2220,7 +2696,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>1008259</v>
       </c>
       <c r="C13" t="n">
         <v>1</v>
@@ -2252,7 +2728,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>1008259</v>
       </c>
       <c r="C15" t="n">
         <v>1</v>
@@ -2268,7 +2744,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>-1804540</v>
       </c>
       <c r="C16" t="n">
         <v>1</v>
@@ -2284,7 +2760,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>7691156</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
@@ -2316,7 +2792,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>5212013</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
@@ -2348,7 +2824,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>-357493</v>
       </c>
       <c r="C21" t="n">
         <v>1</v>
@@ -2364,7 +2840,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>-1167323</v>
       </c>
       <c r="C22" t="n">
         <v>1</v>
@@ -2396,13 +2872,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>-0.035</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>-0.035</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>-0.035</v>
       </c>
     </row>
   </sheetData>
@@ -2448,13 +2924,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2.95</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2.95</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="3">
@@ -2464,13 +2940,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>128071304</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>128071304</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>128071304</v>
       </c>
     </row>
     <row r="4">
@@ -2480,13 +2956,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>198363000</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>190898000</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>330977000</v>
       </c>
     </row>
     <row r="5">
@@ -2496,13 +2972,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>-15830000</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>19762000</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>97998000</v>
       </c>
     </row>
     <row r="6">
@@ -2512,13 +2988,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>-361205000</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>-293810000</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>-183256000</v>
       </c>
     </row>
     <row r="7">
@@ -2528,13 +3004,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>-307049000</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>-234875000</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>-284320000</v>
       </c>
     </row>
     <row r="8">
@@ -2544,13 +3020,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>-361205000</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>-293810000</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>-183256000</v>
       </c>
     </row>
     <row r="9">
@@ -2560,13 +3036,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>188278000</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>326703000</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>361498000</v>
       </c>
     </row>
     <row r="10">
@@ -2576,13 +3052,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>4341000</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>3356000</v>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>6284000</v>
       </c>
     </row>
     <row r="11">
@@ -2592,13 +3068,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>282487000</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>1228692000</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>1111136000</v>
       </c>
     </row>
     <row r="12">
@@ -2608,13 +3084,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>4297445000</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>4585394000</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>3465390000</v>
       </c>
     </row>
     <row r="13">
@@ -2624,13 +3100,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>627451000</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>870265000</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>1108171000</v>
       </c>
     </row>
     <row r="14">
@@ -2640,13 +3116,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>1291763000</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>720044000</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>799051000</v>
       </c>
     </row>
     <row r="15">
@@ -2656,13 +3132,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>2408207000</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>1877297000</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>2054191000</v>
       </c>
     </row>
     <row r="16">
@@ -2672,13 +3148,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>-1785517000</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>-1232991000</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>-879393000</v>
       </c>
     </row>
     <row r="17">
@@ -2688,13 +3164,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>4297445000</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>4585394000</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>3465390000</v>
       </c>
     </row>
     <row r="18">
@@ -2752,13 +3228,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>-195347000</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>-38591000</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>26732000</v>
       </c>
     </row>
     <row r="22">
@@ -2768,13 +3244,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>-700925000</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>-764396000</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>-289103000</v>
       </c>
     </row>
     <row r="23">
@@ -2784,13 +3260,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>56353000</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>45016000</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>89453000</v>
       </c>
     </row>
     <row r="24">
@@ -2800,13 +3276,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>-2.064</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>-2.064</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>-2.064</v>
       </c>
     </row>
   </sheetData>
@@ -2852,13 +3328,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>0.0309</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0.0309</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.0309</v>
       </c>
     </row>
     <row r="3">
@@ -2868,13 +3344,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>21118728</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>21118728</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>21118728</v>
       </c>
     </row>
     <row r="4">
@@ -2884,13 +3360,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>5310000</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>4875000</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>3289000</v>
       </c>
     </row>
     <row r="5">
@@ -2900,13 +3376,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>3385000</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>3789000</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3289000</v>
       </c>
     </row>
     <row r="6">
@@ -2916,13 +3392,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>-7872000</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>-9165000</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>-7599000</v>
       </c>
     </row>
     <row r="7">
@@ -2932,13 +3408,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>-9520000</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>-11415000</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>-12917000</v>
       </c>
     </row>
     <row r="8">
@@ -2948,13 +3424,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>-7872000</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>-9165000</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>-7599000</v>
       </c>
     </row>
     <row r="9">
@@ -2964,13 +3440,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>1014000</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>1527000</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>1274000</v>
       </c>
     </row>
     <row r="10">
@@ -2980,10 +3456,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>1976000</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>42000</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
@@ -2996,13 +3472,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>4982000</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>5461000</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>10311000</v>
       </c>
     </row>
     <row r="12">
@@ -3012,13 +3488,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>14428000</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>16307000</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>15050000</v>
       </c>
     </row>
     <row r="13">
@@ -3028,13 +3504,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>3940000</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>7182000</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>3641000</v>
       </c>
     </row>
     <row r="14">
@@ -3044,13 +3520,13 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>2909000</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>715000</v>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>1709000</v>
       </c>
     </row>
     <row r="15">
@@ -3060,13 +3536,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>9354000</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>7909000</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>8986000</v>
       </c>
     </row>
     <row r="16">
@@ -3076,13 +3552,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>-48396000</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>-38571000</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>-27156000</v>
       </c>
     </row>
     <row r="17">
@@ -3092,13 +3568,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>14428000</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>16307000</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>15050000</v>
       </c>
     </row>
     <row r="18">
@@ -3124,13 +3600,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>2722000</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>5438000</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>8345000</v>
       </c>
     </row>
     <row r="20">
@@ -3156,13 +3632,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>-5279000</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>-6081000</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>-4251000</v>
       </c>
     </row>
     <row r="22">
@@ -3172,13 +3648,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>-757000</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>-3997000</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>-2408000</v>
       </c>
     </row>
     <row r="23">
@@ -3188,13 +3664,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>2732000</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>2471000</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>485000</v>
       </c>
     </row>
     <row r="24">
@@ -3204,13 +3680,13 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>-0.015</v>
       </c>
       <c r="C24" t="n">
-        <v>1</v>
+        <v>-0.015</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>-0.015</v>
       </c>
     </row>
   </sheetData>
@@ -3256,13 +3732,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2.07</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2.07</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>2.07</v>
       </c>
     </row>
     <row r="3">
@@ -3272,13 +3748,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>257735696</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>257735696</v>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>257735696</v>
       </c>
     </row>
     <row r="4">
@@ -3320,13 +3796,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>-3823863</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>-913236</v>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>-46335</v>
       </c>
     </row>
     <row r="7">
@@ -3336,13 +3812,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>-4207030</v>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>-889732</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>-76219</v>
       </c>
     </row>
     <row r="8">
@@ -3352,13 +3828,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>-3823863</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>-913236</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>-46335</v>
       </c>
     </row>
     <row r="9">
@@ -3368,13 +3844,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>262943</v>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>89599</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>775</v>
       </c>
     </row>
     <row r="10">
@@ -3400,13 +3876,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>2953197</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>251646</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>104877</v>
       </c>
     </row>
     <row r="12">
@@ -3416,13 +3892,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>9639681</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>1611322</v>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>277596</v>
       </c>
     </row>
     <row r="13">
@@ -3432,13 +3908,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>142915</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>68221</v>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>5625</v>
       </c>
     </row>
     <row r="14">
@@ -3464,13 +3940,13 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>142915</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>73088</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>23057</v>
       </c>
     </row>
     <row r="16">
@@ -3480,13 +3956,13 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>-5141223</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>-934193</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>-44461</v>
       </c>
     </row>
     <row r="17">
@@ -3496,13 +3972,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>9639681</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>1611322</v>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>277596</v>
       </c>
     </row>
     <row r="18">
@@ -3528,13 +4004,13 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>8948055</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>597552</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>524572</v>
       </c>
     </row>
     <row r="20">
@@ -3560,13 +4036,13 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>-3031810</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>-223657</v>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>-60862</v>
       </c>
     </row>
     <row r="22">
@@ -3576,13 +4052,13 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>-2051359</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>-293181</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>-224510</v>
       </c>
     </row>
     <row r="23">
@@ -3592,13 +4068,417 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>5056</v>
       </c>
       <c r="C23" t="n">
-        <v>1</v>
+        <v>436324</v>
       </c>
       <c r="D23" t="n">
-        <v>1</v>
+        <v>436324</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>eps</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Current</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>1YA</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>2YA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>sharePrice</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4.35</v>
+      </c>
+      <c r="C2" t="n">
+        <v>4.35</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4.35</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>marketCap</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>60638128</v>
+      </c>
+      <c r="C3" t="n">
+        <v>60638128</v>
+      </c>
+      <c r="D3" t="n">
+        <v>60638128</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>totalRevenue</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>413854000</v>
+      </c>
+      <c r="C4" t="n">
+        <v>521695000</v>
+      </c>
+      <c r="D4" t="n">
+        <v>436165000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>grossProfit</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>80392000</v>
+      </c>
+      <c r="C5" t="n">
+        <v>115299000</v>
+      </c>
+      <c r="D5" t="n">
+        <v>103833000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>operatingIncome</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-63286000</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-58966000</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-95993000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>netIncome</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-97418000</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-88796000</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-120589000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>ebit</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-63286000</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-58966000</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-95993000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>netReceivables</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>57566000</v>
+      </c>
+      <c r="C9" t="n">
+        <v>80618000</v>
+      </c>
+      <c r="D9" t="n">
+        <v>76647000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>inventory</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>13565000</v>
+      </c>
+      <c r="C10" t="n">
+        <v>15861000</v>
+      </c>
+      <c r="D10" t="n">
+        <v>20942000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>currentAssets</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>101592000</v>
+      </c>
+      <c r="C11" t="n">
+        <v>158498000</v>
+      </c>
+      <c r="D11" t="n">
+        <v>186803000</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>totalAssets</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>347870000</v>
+      </c>
+      <c r="C12" t="n">
+        <v>443174000</v>
+      </c>
+      <c r="D12" t="n">
+        <v>529121000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>currentLiabilities</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>102334000</v>
+      </c>
+      <c r="C13" t="n">
+        <v>103464000</v>
+      </c>
+      <c r="D13" t="n">
+        <v>103776000</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>longTermDebt</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>238826000</v>
+      </c>
+      <c r="C14" t="n">
+        <v>241079000</v>
+      </c>
+      <c r="D14" t="n">
+        <v>243103000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>totalLiabilities</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>399123000</v>
+      </c>
+      <c r="C15" t="n">
+        <v>397654000</v>
+      </c>
+      <c r="D15" t="n">
+        <v>400438000</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>retainedEarnings</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-317047000</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-219629000</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-130833000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>liabilitiesAndEquity</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>347870000</v>
+      </c>
+      <c r="C17" t="n">
+        <v>443174000</v>
+      </c>
+      <c r="D17" t="n">
+        <v>529121000</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>dividends</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>shareIssuance</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D19" t="n">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>shareBuyback</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>-39000</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-280000</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-697000</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>operatingCashFlow</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-29011000</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-1845000</v>
+      </c>
+      <c r="D21" t="n">
+        <v>-51367000</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>capitalExpenditure</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-18302000</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-37535000</v>
+      </c>
+      <c r="D22" t="n">
+        <v>-16079000</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>depreciation</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>57137000</v>
+      </c>
+      <c r="C23" t="n">
+        <v>82803000</v>
+      </c>
+      <c r="D23" t="n">
+        <v>84763000</v>
       </c>
     </row>
     <row r="24">

</xml_diff>